<commit_message>
NHA : report v2.2.0 from svn to git (Generic CommonSteps + relooked Conditioned steps)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/hello.xlsx
+++ b/src/test/resources/data/in/hello.xlsx
@@ -64,16 +64,16 @@
     <t>element</t>
   </si>
   <si>
-    <t>-smile</t>
-  </si>
-  <si>
     <t>Jenkins T5</t>
   </si>
   <si>
-    <t>-noExistElement</t>
-  </si>
-  <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>smile</t>
+  </si>
+  <si>
+    <t>noExistElement</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -512,7 +512,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="12">
         <v>43846</v>
@@ -531,7 +531,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="11">
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="11">
@@ -569,7 +569,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="8"/>
@@ -577,7 +577,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>5</v>
@@ -586,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11">

</xml_diff>

<commit_message>
add any CI case for code coverage
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/hello.xlsx
+++ b/src/test/resources/data/in/hello.xlsx
@@ -469,7 +469,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="11">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3"/>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
use en result in hello scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/hello.xlsx
+++ b/src/test/resources/data/in/hello.xlsx
@@ -19,9 +19,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
-    <t>Résultat</t>
-  </si>
-  <si>
     <t>author</t>
   </si>
   <si>
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>element2</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,45 +502,45 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="10">
         <v>43846</v>
@@ -551,19 +551,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -574,19 +574,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -597,19 +597,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -618,19 +618,19 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -640,17 +640,17 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -660,13 +660,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -678,17 +678,17 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>

</xml_diff>